<commit_message>
small changes in all notebook. added poi categories and number of trips per category.
</commit_message>
<xml_diff>
--- a/input/anzhal-Wege-POIKeys.xlsx
+++ b/input/anzhal-Wege-POIKeys.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Ziel/Zweck</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Dienstleistungseinrichtung (z. B. Post. Bank. Friseur)</t>
   </si>
   <si>
-    <t xml:space="preserve">;roofer;electronics_repair;beekeeper;joiner;printer;boatbuilder;distillery;conservator;photographic_laboratory;upholsterer;chimney_sweeper;locksmith;plasterer;clockmaker;cooper;insulation;saddler;cosmeticsun protection;painter;dressmaker;gardenerliquid_gas_appliances;key_cutter;engraver;Make-up Artist;post_office SFX;brewery;metal_construction;car_panel_beater;taxidermist;pastry;interior_work;glass;plumbing;floorer;luthier;picture_frames;printmaker;blacksmith;dryer;aircraftmaker;stonemason;agricultural_engines;leather;tinsmith;pest_control;piano_tuner;watchmaker;goldsmith;scaffolder;cleaning;construction;glass_mosaik;sculptor;parquet_layer;sewing_machine_repair;shoemaker;print_shop;signmaker;toolmaker;exterminator;embroiderer;tailor;furniture_maker;furniture;electrician;printers;shoe_repair;handicraft;carpet_cleaner;basket_maker;atelier;oil_mill;photo_studio;jeweller;optical_components;janitor;confectionery;heating_engineer;interior_decoration;pottery;workshop;wall_draining;hvac;sharpening;carpet_layer;glaziery;pyrotechnician;frame-maker;carpenter;candles;frame_maker;tiler;cabinet_maker;electroplating;photographer;builder;yes;plumber;optician;model;dental_technician;goldsmtih;musical_instrument;caterer;window_construction;maintenance;oem;car_painter;transportation;bookbinder;sun_protection;organ_builder;interior_decorator;grinder;printing;weaver;hatter;glassblowing;</t>
+    <t xml:space="preserve">roofer;electronics_repair;beekeeper;joiner;printer;boatbuilder;distillery;conservator;photographic_laboratory;upholsterer;chimney_sweeper;locksmith;plasterer;clockmaker;cooper;insulation;saddler;cosmeticsun protection;painter;dressmaker;gardenerliquid_gas_appliances;key_cutter;engraver;Make-up Artist;post_office SFX;brewery;metal_construction;car_panel_beater;taxidermist;pastry;interior_work;glass;plumbing;floorer;luthier;picture_frames;printmaker;blacksmith;dryer;aircraftmaker;stonemason;agricultural_engines;leather;tinsmith;pest_control;piano_tuner;watchmaker;goldsmith;scaffolder;cleaning;construction;glass_mosaik;sculptor;parquet_layer;sewing_machine_repair;shoemaker;print_shop;signmaker;toolmaker;exterminator;embroiderer;tailor;furniture_maker;furniture;electrician;printers;shoe_repair;handicraft;carpet_cleaner;basket_maker;atelier;oil_mill;photo_studio;jeweller;optical_components;janitor;confectionery;heating_engineer;interior_decoration;pottery;workshop;wall_draining;hvac;sharpening;carpet_layer;glaziery;pyrotechnician;frame-maker;carpenter;candles;frame_maker;tiler;cabinet_maker;electroplating;photographer;builder;yes;plumber;optician;model;dental_technician;goldsmtih;musical_instrument;caterer;window_construction;maintenance;oem;car_painter;transportation;bookbinder;sun_protection;organ_builder;interior_decorator;grinder;printing;weaver;hatter;glassblowing;</t>
   </si>
   <si>
     <t xml:space="preserve">Kultur. Theater. Kino</t>
@@ -76,22 +76,19 @@
     <t xml:space="preserve">Gaststätte/Kneipe</t>
   </si>
   <si>
-    <t xml:space="preserve">restaurant;biergarten;cafe;pub;bar;icecream;hotel</t>
+    <t xml:space="preserve">restaurant;biergarten;cafe;pub;bar;icecream;hotel;hostel</t>
   </si>
   <si>
     <t xml:space="preserve">Summe Sport Freizeit</t>
   </si>
   <si>
-    <t xml:space="preserve">community_centre;public_bath;stadium;beach_resort;sports_centre;marina;swimming_pool;park;nature_reserve;water_park;attraction;theme_park;zoo;aquarium;lake;pitch;camp_site;caravan_site</t>
+    <t xml:space="preserve">community_centre;public_bath;stadium;beach_resort;sports_centre;marina;swimming_pool;park;nature_reserve;water_park;attraction;theme_park;zoo;aquarium;lake;pitch;camp_site;caravan_site;place_of_worship</t>
   </si>
   <si>
     <t xml:space="preserve">Eigene Wohnung</t>
   </si>
   <si>
     <t xml:space="preserve">Sonstiges Summe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">place_of_worship;hostel</t>
   </si>
   <si>
     <t xml:space="preserve">Ungewichtete Fallzahl</t>
@@ -201,12 +198,12 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.74"/>
@@ -406,13 +403,10 @@
       <c r="D12" s="0" t="n">
         <v>9.4</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>123899</v>
@@ -426,7 +420,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>124418</v>
@@ -443,8 +437,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>